<commit_message>
add new test data
</commit_message>
<xml_diff>
--- a/data_prep/input/global_metainfo/datasets_info.xlsx
+++ b/data_prep/input/global_metainfo/datasets_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisahulsmann/Dropbox/Work/Publications ongoing/2022 Huelsmann CNDD dynamic/analysis/latitudinalCNDD@git/data_prep/input/global_metainfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51771E40-50F2-0A43-A401-9D78A95718A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF36332F-FBC9-1546-94A2-14E6FD83D6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16900" xr2:uid="{EA16E01C-8C44-A748-BD9D-64E1B7A8488F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="20">
   <si>
     <t>yes</t>
   </si>
@@ -68,17 +68,41 @@
     <t>ID</t>
   </si>
   <si>
-    <t>bcione</t>
+    <t>site10</t>
   </si>
   <si>
-    <t>bcitwo</t>
+    <t>site01</t>
+  </si>
+  <si>
+    <t>site02</t>
+  </si>
+  <si>
+    <t>site03</t>
+  </si>
+  <si>
+    <t>site04</t>
+  </si>
+  <si>
+    <t>site05</t>
+  </si>
+  <si>
+    <t>site06</t>
+  </si>
+  <si>
+    <t>site07</t>
+  </si>
+  <si>
+    <t>site08</t>
+  </si>
+  <si>
+    <t>site09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +114,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,7 +167,147 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -488,11 +658,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB612A5-ECE4-5C4B-AA65-C317EDC33AA4}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:A16"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +720,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -573,7 +743,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -592,7 +762,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -611,7 +781,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -630,7 +800,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -649,7 +819,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -668,7 +838,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -687,7 +857,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -710,7 +880,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -729,7 +899,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -748,7 +918,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -767,7 +937,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -786,7 +956,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -805,7 +975,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -822,16 +992,990 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58">
+        <v>7</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G9" xr:uid="{5C5D37EC-F27F-8044-AE80-78EF641C1ED8}"/>
-  <mergeCells count="4">
+  <mergeCells count="18">
     <mergeCell ref="F10:F16"/>
     <mergeCell ref="G10:G16"/>
     <mergeCell ref="F3:F9"/>
     <mergeCell ref="G3:G9"/>
+    <mergeCell ref="F17:F23"/>
+    <mergeCell ref="G17:G23"/>
+    <mergeCell ref="F24:F30"/>
+    <mergeCell ref="G24:G30"/>
+    <mergeCell ref="F31:F37"/>
+    <mergeCell ref="G31:G37"/>
+    <mergeCell ref="F38:F44"/>
+    <mergeCell ref="G38:G44"/>
+    <mergeCell ref="F45:F51"/>
+    <mergeCell ref="G45:G51"/>
+    <mergeCell ref="F52:F58"/>
+    <mergeCell ref="G52:G58"/>
+    <mergeCell ref="F59:F65"/>
+    <mergeCell ref="G59:G65"/>
   </mergeCells>
-  <conditionalFormatting sqref="C17:G1048576 C1:G3 C4:E9 C10:G10 C11:E16">
-    <cfRule type="dataBar" priority="17">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C66:G1048576 C1:G3 C4:E9 C10:G10 C11:E16 C17:G17 C18:E23 C24:G24 C25:E30 C31:G31 C32:E37 C38:G38 C39:E44 C45:G45 C46:E51 C52:G52 C53:E58 C59:G59 C60:E65">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="num" val="$C$2"/>
@@ -845,19 +1989,75 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:G3 C4:E9">
-    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="17" priority="29" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="16" priority="30" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:G10 C11:E16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",C10)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",C10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:G17 C18:E23">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:G24 C25:E30">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",C24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:G31 C32:E37">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",C31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:G38 C39:E44">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:G45 C46:E51">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C45)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",C45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:G52 C53:E58">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",C52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:G59 C60:E65">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C59)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",C10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("yes",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -875,7 +2075,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C17:G1048576 C1:G3 C4:E9 C10:G10 C11:E16</xm:sqref>
+          <xm:sqref>C66:G1048576 C1:G3 C4:E9 C10:G10 C11:E16 C17:G17 C18:E23 C24:G24 C25:E30 C31:G31 C32:E37 C38:G38 C39:E44 C45:G45 C46:E51 C52:G52 C53:E58 C59:G59 C60:E65</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>